<commit_message>
closeness, parallel closeness and performance analysis
</commit_message>
<xml_diff>
--- a/performance/performance_es_2.xlsx
+++ b/performance/performance_es_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F795E-4619-423D-9E68-D703B35F6C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDF5935-8769-4E24-8061-467218C5DA5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="5640" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,10 +438,15 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -493,6 +498,9 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D3">
+        <v>1554.2362387180301</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -569,6 +577,12 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D11">
+        <v>269.693302631378</v>
+      </c>
+      <c r="E11">
+        <v>265.10288429260203</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
performance es 2 modified
</commit_message>
<xml_diff>
--- a/performance/performance_es_2.xlsx
+++ b/performance/performance_es_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDF5935-8769-4E24-8061-467218C5DA5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8335DD9-72F2-4E26-8A25-2B30C16FEC18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,6 +584,9 @@
       <c r="E11">
         <v>265.10288429260203</v>
       </c>
+      <c r="F11">
+        <v>267.00966644287098</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">

</xml_diff>

<commit_message>
performance analysis es2 + aggiunt afile arcangelo mario
</commit_message>
<xml_diff>
--- a/performance/performance_es_2.xlsx
+++ b/performance/performance_es_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\SNA\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9345BF-CEFD-4926-A5CD-35217C5AF4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF724C-1622-4055-BA0B-1B366D585B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="1960" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,6 +493,9 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D2">
+        <v>9.2720985412597601E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">

</xml_diff>